<commit_message>
Made changes to sim
kimiya play around with the values
</commit_message>
<xml_diff>
--- a/Simulations/Piezo Calculations.xlsx
+++ b/Simulations/Piezo Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pinger-V2\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5EF0AA-72FF-4E2C-9EDF-C4A6A3C41634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C213E-D221-41A9-92EE-469983216DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33C40750-07C3-4F62-A2BA-357740D35B20}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{33C40750-07C3-4F62-A2BA-357740D35B20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,14 +413,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42ADA57-B79C-423C-AB98-8E4A2FE9B66D}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>